<commit_message>
fixed a typo on risk assessment
</commit_message>
<xml_diff>
--- a/risk_assessment.xlsx
+++ b/risk_assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ddb5747ff8fb28c/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sajis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B603126-AEF2-42D7-B500-9C459F5B2009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2880D0-F0A8-4C15-AB6F-D2235E84C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6405" yWindow="4448" windowWidth="13133" windowHeight="10522" xr2:uid="{539CB195-4B53-46A4-935F-AED5F56D011C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{539CB195-4B53-46A4-935F-AED5F56D011C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Description</t>
   </si>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40470877-E460-4E98-8029-0BC173761B42}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -778,9 +778,6 @@
       <c r="G9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>